<commit_message>
Adicionei alguns itens na planilha do backlog
</commit_message>
<xml_diff>
--- a/BACKLOG - Truticultura.xlsx
+++ b/BACKLOG - Truticultura.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjetoPI-Truta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjetoPI-Truta\projeto-pi-truta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732A5ADA-8BEC-470A-8EBE-6FC64D483BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C339461-C792-4D02-BC63-5475AF9A7A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -665,57 +665,6 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -725,6 +674,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -733,6 +688,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1116,7 +1116,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1132,15 +1132,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1153,14 +1153,14 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="46" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="47"/>
+      <c r="E2" s="42"/>
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1176,13 +1176,13 @@
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="56">
-        <v>1</v>
-      </c>
-      <c r="C3" s="57" t="s">
+      <c r="B3" s="39">
+        <v>1</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="7">
@@ -1194,9 +1194,9 @@
       <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="44"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="57"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="7">
         <v>2</v>
       </c>
@@ -1206,47 +1206,53 @@
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="6">
         <v>2</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="44"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="6">
         <v>3</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="44"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="6">
         <v>4</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="44"/>
-      <c r="B8" s="40">
+      <c r="A8" s="52"/>
+      <c r="B8" s="48">
         <v>5</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="43" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="8">
@@ -1263,9 +1269,9 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="44"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="59"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="9">
         <v>2</v>
       </c>
@@ -1280,9 +1286,9 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="44"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="59"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="10">
         <v>3</v>
       </c>
@@ -1297,9 +1303,9 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="44"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="59"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="7">
         <v>4</v>
       </c>
@@ -1314,9 +1320,9 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="45"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="60"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="45"/>
       <c r="D12" s="7">
         <v>5</v>
       </c>
@@ -1346,7 +1352,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="54" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="18">
@@ -1364,7 +1370,7 @@
       <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="48"/>
+      <c r="A15" s="54"/>
       <c r="B15" s="18">
         <v>2</v>
       </c>
@@ -1380,7 +1386,7 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
+      <c r="A16" s="55"/>
       <c r="B16" s="18">
         <v>3</v>
       </c>
@@ -1398,7 +1404,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="56" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="20">
@@ -1407,36 +1413,42 @@
       <c r="C17" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="21"/>
+      <c r="D17" s="21">
+        <v>1</v>
+      </c>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="51"/>
+      <c r="A18" s="57"/>
       <c r="B18" s="20">
         <v>2</v>
       </c>
       <c r="C18" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="21"/>
+      <c r="D18" s="21">
+        <v>1</v>
+      </c>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="52"/>
+      <c r="A19" s="58"/>
       <c r="B19" s="20">
         <v>3</v>
       </c>
       <c r="C19" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="21"/>
+      <c r="D19" s="21">
+        <v>1</v>
+      </c>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="59" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="23">
@@ -1445,24 +1457,28 @@
       <c r="C20" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="24"/>
+      <c r="D20" s="24">
+        <v>1</v>
+      </c>
       <c r="E20" s="25"/>
       <c r="F20" s="25"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="23">
         <v>2</v>
       </c>
       <c r="C21" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="24"/>
+      <c r="D21" s="24">
+        <v>1</v>
+      </c>
       <c r="E21" s="25"/>
       <c r="F21" s="25"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="46" t="s">
         <v>43</v>
       </c>
       <c r="B22" s="26">
@@ -1471,29 +1487,28 @@
       <c r="C22" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="27"/>
+      <c r="D22" s="27">
+        <v>1</v>
+      </c>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="39"/>
+      <c r="A23" s="47"/>
       <c r="B23" s="26">
         <v>2</v>
       </c>
       <c r="C23" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="27"/>
+      <c r="D23" s="27">
+        <v>1</v>
+      </c>
       <c r="E23" s="28"/>
       <c r="F23" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="C8:C12"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="B8:B12"/>
     <mergeCell ref="A3:A12"/>
@@ -1501,6 +1516,11 @@
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="C8:C12"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="IMPORTANTE">

</xml_diff>

<commit_message>
Correção do BackLog e Atualização de Projeto
</commit_message>
<xml_diff>
--- a/BACKLOG - Truticultura.xlsx
+++ b/BACKLOG - Truticultura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\OneDrive\Área de Trabalho\Projeto\projeto-pi-truta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBE9293-F968-4E1C-9D85-F7DE23018EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAF78C2-C81B-47AA-8904-11CC1F7C79CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BACKLOG" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="85">
   <si>
     <t>REQUISITOS PARA A TRUTICULTURA - BACKLOG</t>
   </si>
@@ -269,9 +269,6 @@
     <t>Inserção de tabelas - dados do negócio</t>
   </si>
   <si>
-    <t>se vira</t>
-  </si>
-  <si>
     <t>Estruturação de tabelas com  dados do negócio, qtde de peixes, etc.</t>
   </si>
   <si>
@@ -281,9 +278,6 @@
     <t>Organizar o Backlog para gerenciamento do projeto</t>
   </si>
   <si>
-    <t>"Depois tomba." MARCOS, PROFESSOR</t>
-  </si>
-  <si>
     <t xml:space="preserve">Alocação de Recursos Humanos </t>
   </si>
   <si>
@@ -308,12 +302,6 @@
     <t>Criação de logotipo</t>
   </si>
   <si>
-    <t>Troust Solution</t>
-  </si>
-  <si>
-    <t>Desenhinho da maria</t>
-  </si>
-  <si>
     <t>Diagrama de Solução (Aula 3 TI)</t>
   </si>
   <si>
@@ -323,7 +311,40 @@
     <t>IMPORTANTE</t>
   </si>
   <si>
-    <t>XPTO</t>
+    <t>Diretório para monitoramento e versionamento do projeto</t>
+  </si>
+  <si>
+    <t>Configurar acesso dos membros da equipe</t>
+  </si>
+  <si>
+    <t>Desenvolvimento de logotipo adequado para a solução oferecida</t>
+  </si>
+  <si>
+    <t>Estabelecimento de parâmetros como missão, solução, etc.</t>
+  </si>
+  <si>
+    <t>Página personalizada com dados obtidos do sensor(es) de cada usuário</t>
+  </si>
+  <si>
+    <t>Sistematizar o BackLog na plataforma Trello</t>
+  </si>
+  <si>
+    <t>Diagramar a solução oferecida, destacando a importância do sensor e do monitoramento</t>
+  </si>
+  <si>
+    <t>Plataforma de trabalho essencial para o desenvolvimento do Banco de Dados</t>
+  </si>
+  <si>
+    <t>Scripts apropriados para inserir dados</t>
+  </si>
+  <si>
+    <t>Scripts apropriados para retornar dados</t>
+  </si>
+  <si>
+    <t>Elaborar linhas de código em MySQL para inserir dados nas tabelas adequadas.</t>
+  </si>
+  <si>
+    <t>Elaborar linhas de código em MySQL para selecionar dados das tabelas adequadas.</t>
   </si>
 </sst>
 </file>
@@ -761,56 +782,8 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -821,6 +794,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -830,23 +809,65 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1235,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA332929-9E23-4A6D-B7F7-7ABCC9990125}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1246,21 +1267,22 @@
     <col min="3" max="3" width="43" style="31" customWidth="1"/>
     <col min="4" max="4" width="2" style="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="70.109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="73.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="4"/>
+    <col min="8" max="8" width="10.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1273,14 +1295,14 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="46" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="47"/>
+      <c r="E2" s="43"/>
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1296,13 +1318,13 @@
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="56">
-        <v>1</v>
-      </c>
-      <c r="C3" s="57" t="s">
+      <c r="B3" s="40">
+        <v>1</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="7">
@@ -1312,16 +1334,16 @@
         <v>8</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="44"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="57"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="41"/>
       <c r="D4" s="7">
         <v>2</v>
       </c>
@@ -1329,14 +1351,14 @@
         <v>9</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
+      <c r="A5" s="55"/>
       <c r="B5" s="6">
         <v>2</v>
       </c>
@@ -1347,17 +1369,17 @@
         <v>1</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="44"/>
+      <c r="A6" s="55"/>
       <c r="B6" s="6">
         <v>3</v>
       </c>
@@ -1368,59 +1390,59 @@
         <v>1</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="44"/>
+      <c r="A7" s="55"/>
       <c r="B7" s="6">
         <v>4</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="47" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F7" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="44"/>
-      <c r="B8" s="64"/>
-      <c r="C8" s="66"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="48"/>
       <c r="D8" s="8">
         <v>2</v>
       </c>
       <c r="E8" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="44"/>
-      <c r="B9" s="40">
+      <c r="A9" s="55"/>
+      <c r="B9" s="51">
         <v>5</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="44" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="8">
@@ -1437,9 +1459,9 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="44"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="59"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="9">
         <v>2</v>
       </c>
@@ -1454,9 +1476,9 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="44"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="59"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="10">
         <v>3</v>
       </c>
@@ -1471,9 +1493,9 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="44"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="59"/>
+      <c r="A12" s="55"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="45"/>
       <c r="D12" s="7">
         <v>4</v>
       </c>
@@ -1488,9 +1510,9 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="45"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="60"/>
+      <c r="A13" s="56"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="7">
         <v>5</v>
       </c>
@@ -1524,11 +1546,11 @@
         <v>27</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="65" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="67">
@@ -1544,31 +1566,31 @@
         <v>30</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="48"/>
+      <c r="A16" s="65"/>
       <c r="B16" s="68"/>
       <c r="C16" s="33"/>
       <c r="D16" s="19">
         <v>2</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="48"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="65"/>
       <c r="B17" s="18">
         <v>2</v>
       </c>
@@ -1582,14 +1604,14 @@
         <v>32</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
+      <c r="A18" s="65"/>
       <c r="B18" s="67">
         <v>3</v>
       </c>
@@ -1609,28 +1631,28 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
+    <row r="19" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="66"/>
       <c r="B19" s="68"/>
       <c r="C19" s="33"/>
       <c r="D19" s="19">
         <v>2</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="61">
+      <c r="B20" s="62">
         <v>1</v>
       </c>
       <c r="C20" s="34" t="s">
@@ -1643,15 +1665,15 @@
         <v>54</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="51"/>
-      <c r="B21" s="62"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="63"/>
       <c r="C21" s="34"/>
       <c r="D21" s="21">
         <v>2</v>
@@ -1667,8 +1689,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="51"/>
-      <c r="B22" s="62"/>
+      <c r="A22" s="58"/>
+      <c r="B22" s="63"/>
       <c r="C22" s="34"/>
       <c r="D22" s="21">
         <v>3</v>
@@ -1677,15 +1699,15 @@
         <v>58</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="51"/>
-      <c r="B23" s="63"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="64"/>
       <c r="C23" s="34"/>
       <c r="D23" s="21">
         <v>4</v>
@@ -1694,14 +1716,14 @@
         <v>57</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="51"/>
+      <c r="A24" s="58"/>
       <c r="B24" s="20">
         <v>2</v>
       </c>
@@ -1712,17 +1734,17 @@
         <v>1</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="52"/>
+      <c r="A25" s="59"/>
       <c r="B25" s="20">
         <v>3</v>
       </c>
@@ -1733,17 +1755,17 @@
         <v>1</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="53" t="s">
+      <c r="A26" s="60" t="s">
         <v>40</v>
       </c>
       <c r="B26" s="23">
@@ -1766,7 +1788,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
+      <c r="A27" s="61"/>
       <c r="B27" s="23">
         <v>2</v>
       </c>
@@ -1787,7 +1809,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="49" t="s">
         <v>43</v>
       </c>
       <c r="B28" s="26">
@@ -1806,11 +1828,11 @@
         <v>47</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="39"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="26">
         <v>2</v>
       </c>
@@ -1827,17 +1849,11 @@
         <v>49</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="C7:C8"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="A3:A13"/>
@@ -1848,6 +1864,12 @@
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="IMPORTANTE">

</xml_diff>